<commit_message>
fix: change sample query
</commit_message>
<xml_diff>
--- a/data/example0.2.xlsx
+++ b/data/example0.2.xlsx
@@ -8,19 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\project\vdt\xlsx_chatbot\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8D25898-5F6F-40AB-9859-CE1F999B13D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{606A7C81-ED1F-47DC-AAE5-EEFCB4F8C6E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="45">
   <si>
     <t>Cà phê</t>
   </si>
@@ -86,13 +89,82 @@
   </si>
   <si>
     <t>Ý</t>
+  </si>
+  <si>
+    <t>Doanh nghiệp</t>
+  </si>
+  <si>
+    <t>Cà phê Sữa</t>
+  </si>
+  <si>
+    <t>100k</t>
+  </si>
+  <si>
+    <t>200k</t>
+  </si>
+  <si>
+    <t>300k</t>
+  </si>
+  <si>
+    <t>400k</t>
+  </si>
+  <si>
+    <t>500k</t>
+  </si>
+  <si>
+    <t>600k</t>
+  </si>
+  <si>
+    <t>Có đá</t>
+  </si>
+  <si>
+    <t>Không</t>
+  </si>
+  <si>
+    <t>Cà phê muối</t>
+  </si>
+  <si>
+    <t>Họ và tên</t>
+  </si>
+  <si>
+    <t>Lớp</t>
+  </si>
+  <si>
+    <t>Trường</t>
+  </si>
+  <si>
+    <t>ABC</t>
+  </si>
+  <si>
+    <t>XYZ</t>
+  </si>
+  <si>
+    <t>DEF</t>
+  </si>
+  <si>
+    <t>IJK</t>
+  </si>
+  <si>
+    <t>MNP</t>
+  </si>
+  <si>
+    <t>UVX</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>Giá 2025</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -113,16 +185,47 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B0F0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B0F0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -171,33 +274,87 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -505,230 +662,231 @@
   </sheetPr>
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView zoomScale="92" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.6640625" customWidth="1"/>
+    <col min="1" max="1" width="13.44140625" customWidth="1"/>
+    <col min="2" max="2" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.77734375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="5"/>
+      <c r="F1" s="18"/>
     </row>
     <row r="2" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="1" t="s">
+      <c r="A2" s="16"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="20" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3" t="s">
+      <c r="A4" s="21"/>
+      <c r="B4" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3" t="s">
+      <c r="A5" s="21"/>
+      <c r="B5" s="21"/>
+      <c r="C5" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3" t="s">
+      <c r="A6" s="21"/>
+      <c r="B6" s="21"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3" t="s">
+      <c r="A7" s="21"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3" t="s">
+      <c r="A8" s="21"/>
+      <c r="B8" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3" t="s">
+      <c r="C8" s="21"/>
+      <c r="D8" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3" t="s">
+      <c r="A9" s="21"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="D10" s="3" t="s">
+      <c r="A10" s="21"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
     </row>
     <row r="11" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3" t="s">
+      <c r="A11" s="21"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
     </row>
     <row r="12" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3" t="s">
+      <c r="A12" s="21"/>
+      <c r="B12" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
     </row>
     <row r="13" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3" t="s">
+      <c r="A13" s="21"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
     </row>
     <row r="14" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3" t="s">
+      <c r="A14" s="21"/>
+      <c r="B14" s="21"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
     </row>
     <row r="15" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3" t="s">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
     </row>
     <row r="16" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3" t="s">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
     </row>
     <row r="17" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3" t="s">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
     </row>
     <row r="18" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
     </row>
     <row r="19" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3" t="s">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
     </row>
     <row r="20" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3" t="s">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -740,4 +898,414 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23219E73-F7A8-43CC-93DE-6FDE163A48D1}">
+  <dimension ref="A1:D20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D20" sqref="A1:D20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="10"/>
+      <c r="B2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="5"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="5"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="5"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="5"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="5"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="5"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="5"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="5"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="6"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="5"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="6"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="5"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="6"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="5"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="6"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="5"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="6"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="5"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="6"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="5"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="6"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="5"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="5"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="6"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="5"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="6"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:D1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD31CD95-C4A2-44FC-9927-2CD285822710}">
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="6">
+        <v>1</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="6">
+        <v>2</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="8">
+        <v>3</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="6">
+        <v>4</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" s="6">
+        <v>5</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="6">
+        <v>6</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="6"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E2F2C03-E116-4898-81EA-0961E23D14A0}">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>